<commit_message>
change tel nr to vw in templates
</commit_message>
<xml_diff>
--- a/cg/apps/invoice/templates/KI_pool_invoice.xlsx
+++ b/cg/apps/invoice/templates/KI_pool_invoice.xlsx
@@ -76,9 +76,6 @@
     <t>Telefon</t>
   </si>
   <si>
-    <t>08-5248 1545</t>
-  </si>
-  <si>
     <t>Till</t>
   </si>
   <si>
@@ -119,6 +116,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>073-338 63 41</t>
   </si>
 </sst>
 </file>
@@ -551,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z3315"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -857,7 +857,7 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -913,7 +913,7 @@
     </row>
     <row r="12" spans="1:26" ht="22.5" customHeight="1">
       <c r="A12" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -1007,7 +1007,7 @@
     </row>
     <row r="15" spans="1:26" ht="22.5" customHeight="1">
       <c r="A15" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5" t="s">
@@ -1039,7 +1039,7 @@
     </row>
     <row r="16" spans="1:26" ht="22.5" customHeight="1">
       <c r="A16" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5" t="s">
@@ -1071,7 +1071,7 @@
     </row>
     <row r="17" spans="1:26" ht="22.5" customHeight="1">
       <c r="A17" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5" t="s">
@@ -1131,7 +1131,7 @@
     </row>
     <row r="19" spans="1:26" ht="22.5" customHeight="1">
       <c r="A19" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="20" spans="1:26" ht="22.5" customHeight="1">
       <c r="A20" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5" t="s">
@@ -1249,29 +1249,29 @@
     </row>
     <row r="23" spans="1:26" ht="22.5" customHeight="1">
       <c r="A23" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" s="22"/>
       <c r="C23" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="22" t="s">
+      <c r="E23" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E23" s="22" t="s">
+      <c r="F23" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="F23" s="29" t="s">
+      <c r="G23" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="G23" s="29" t="s">
+      <c r="H23" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="H23" s="30" t="s">
+      <c r="I23" s="30" t="s">
         <v>31</v>
-      </c>
-      <c r="I23" s="30" t="s">
-        <v>32</v>
       </c>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>

</xml_diff>

<commit_message>
change contact (#3690) (patch)
change invoice contact
</commit_message>
<xml_diff>
--- a/cg/apps/invoice/templates/KI_pool_invoice.xlsx
+++ b/cg/apps/invoice/templates/KI_pool_invoice.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10107"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isakohlsson/dev/cg/cg/apps/invoice/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christian/Documents/clinicalGenomics/cg/cg/apps/invoice/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561CF99E-AE14-A34F-8F29-F6D96101BBA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC3DEF9-34E1-6F4D-927E-B7F554680798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Faktura" sheetId="1" r:id="rId1"/>
@@ -118,13 +118,13 @@
     <t>Total</t>
   </si>
   <si>
-    <t>08-524 860 53</t>
+    <t>Anna Zetterlund</t>
   </si>
   <si>
-    <t>Anna Gellerbring</t>
+    <t>anna.zetterlund@scilifelab.se</t>
   </si>
   <si>
-    <t>anna.gellerbring@scilifelab.se</t>
+    <t>(+46) 701523463</t>
   </si>
 </sst>
 </file>
@@ -265,7 +265,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -343,6 +343,9 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -356,7 +359,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -577,15 +580,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z3315"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11.1640625" customWidth="1"/>
     <col min="2" max="2" width="21.1640625" customWidth="1"/>
-    <col min="3" max="5" width="11.1640625" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" customWidth="1"/>
+    <col min="4" max="5" width="11.1640625" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" customWidth="1"/>
     <col min="7" max="7" width="7.6640625" customWidth="1"/>
     <col min="8" max="8" width="9.5" customWidth="1"/>
@@ -594,10 +598,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
+      <c r="B1" s="31"/>
       <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
@@ -630,10 +634,10 @@
       <c r="Z1" s="7"/>
     </row>
     <row r="2" spans="1:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="30"/>
+      <c r="B2" s="31"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5" t="s">
@@ -819,7 +823,7 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -850,8 +854,8 @@
         <v>14</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="34" t="s">
-        <v>32</v>
+      <c r="C9" s="29" t="s">
+        <v>31</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
@@ -882,8 +886,8 @@
         <v>15</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="5" t="s">
-        <v>30</v>
+      <c r="C10" s="35" t="s">
+        <v>32</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -35640,7 +35644,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -35654,10 +35660,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
+      <c r="B1" s="31"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -35670,10 +35676,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="30"/>
+      <c r="B2" s="31"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3" t="s">

</xml_diff>